<commit_message>
Added IC-7300 documentation added power control testing info fixed LCD display dropped characters - decreased I2C bus speed to 50KHz Tested with Rev B controller changed station selection to be a #def in config.h file, from master list in stations.h
</commit_message>
<xml_diff>
--- a/Docs/misc/LCD_layout.xlsx
+++ b/Docs/misc/LCD_layout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
   <si>
     <t>w</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X </t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -516,7 +528,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -603,6 +615,15 @@
       <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1">
       <c r="A3" s="2">
@@ -815,7 +836,50 @@
       </c>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1"/>
-    <row r="15" spans="1:17" s="1" customFormat="1"/>
+    <row r="15" spans="1:17" s="1" customFormat="1">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="16" spans="1:17" s="1" customFormat="1"/>
     <row r="17" s="1" customFormat="1"/>
     <row r="18" s="1" customFormat="1"/>

</xml_diff>

<commit_message>
add eeprom util, labels, read slot ID from EEPROM, update for VE8AT deployment
</commit_message>
<xml_diff>
--- a/Docs/misc/LCD_layout.xlsx
+++ b/Docs/misc/LCD_layout.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MENU" sheetId="2" r:id="rId1"/>
+    <sheet name="OPER" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="34">
   <si>
     <t>w</t>
   </si>
@@ -115,6 +116,12 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -171,8 +178,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -189,13 +200,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -528,6 +543,246 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="17" width="4.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="32" customHeight="1">
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1"/>
+    <row r="5" spans="1:17" s="1" customFormat="1"/>
+    <row r="6" spans="1:17" s="1" customFormat="1"/>
+    <row r="7" spans="1:17" s="1" customFormat="1">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="1" customFormat="1">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="1" customFormat="1"/>
+    <row r="10" spans="1:17" s="1" customFormat="1">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="1" customFormat="1"/>
+    <row r="12" spans="1:17" s="1" customFormat="1"/>
+    <row r="13" spans="1:17" s="1" customFormat="1">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" s="1" customFormat="1"/>
+    <row r="15" spans="1:17" s="1" customFormat="1">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="1" customFormat="1"/>
+    <row r="17" s="1" customFormat="1"/>
+    <row r="18" s="1" customFormat="1"/>
+    <row r="19" s="1" customFormat="1"/>
+    <row r="20" s="1" customFormat="1"/>
+    <row r="21" s="1" customFormat="1"/>
+    <row r="22" s="1" customFormat="1"/>
+    <row r="23" s="1" customFormat="1"/>
+    <row r="24" s="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
code clean up. added SKIP menu item
</commit_message>
<xml_diff>
--- a/Docs/misc/LCD_layout.xlsx
+++ b/Docs/misc/LCD_layout.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="24240" yWindow="7900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MENU" sheetId="2" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="44">
   <si>
     <t>w</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -118,10 +115,43 @@
     <t>B</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>U</t>
+    <t>v</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -543,7 +573,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -607,157 +637,153 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1"/>
     <row r="5" spans="1:17" s="1" customFormat="1"/>
-    <row r="6" spans="1:17" s="1" customFormat="1"/>
+    <row r="6" spans="1:17" s="1" customFormat="1">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="7" spans="1:17" s="1" customFormat="1">
-      <c r="A7" s="2">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>4</v>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="P7" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1">
-      <c r="A8" s="2">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:17" s="1" customFormat="1"/>
     <row r="10" spans="1:17" s="1" customFormat="1">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1"/>
     <row r="12" spans="1:17" s="1" customFormat="1"/>
-    <row r="13" spans="1:17" s="1" customFormat="1">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="13" spans="1:17" s="1" customFormat="1"/>
     <row r="14" spans="1:17" s="1" customFormat="1"/>
-    <row r="15" spans="1:17" s="1" customFormat="1">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="15" spans="1:17" s="1" customFormat="1"/>
     <row r="16" spans="1:17" s="1" customFormat="1"/>
     <row r="17" s="1" customFormat="1"/>
     <row r="18" s="1" customFormat="1"/>
@@ -783,7 +809,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -847,37 +873,49 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J2" s="1">
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1">
@@ -885,52 +923,52 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1"/>
@@ -941,52 +979,52 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="J7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1"/>
@@ -996,49 +1034,49 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1"/>
@@ -1048,46 +1086,46 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="N13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1"/>
@@ -1096,54 +1134,91 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="M15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="1" customFormat="1"/>
+    <row r="17" spans="1:14" s="1" customFormat="1">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" s="1" customFormat="1"/>
-    <row r="17" s="1" customFormat="1"/>
-    <row r="18" s="1" customFormat="1"/>
-    <row r="19" s="1" customFormat="1"/>
-    <row r="20" s="1" customFormat="1"/>
-    <row r="21" s="1" customFormat="1"/>
-    <row r="22" s="1" customFormat="1"/>
-    <row r="23" s="1" customFormat="1"/>
-    <row r="24" s="1" customFormat="1"/>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="1" customFormat="1"/>
+    <row r="19" spans="1:14" s="1" customFormat="1"/>
+    <row r="20" spans="1:14" s="1" customFormat="1"/>
+    <row r="21" spans="1:14" s="1" customFormat="1"/>
+    <row r="22" spans="1:14" s="1" customFormat="1"/>
+    <row r="23" spans="1:14" s="1" customFormat="1"/>
+    <row r="24" spans="1:14" s="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>